<commit_message>
split and classifier structure fix
</commit_message>
<xml_diff>
--- a/statistiche/counterfactualsLGBM.xlsx
+++ b/statistiche/counterfactualsLGBM.xlsx
@@ -436,77 +436,77 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Release D</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>ER Sepsis Triage</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Release B</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Release A</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>IV Liquid</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ER Registration</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Leucocytes</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Admission NC</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>LacticAcid</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>CRP</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ER Triage</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>IV Antibiotics</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Admission IC</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Release C</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Leucocytes</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Release B</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Release D</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>IV Antibiotics</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Admission NC</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Release A</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>ER Registration</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>ER Triage</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>CRP</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>LacticAcid</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
@@ -542,7 +542,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -560,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -593,7 +593,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -602,31 +602,31 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
@@ -653,7 +653,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -662,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -674,19 +674,19 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="O4" t="n">
         <v>0</v>
@@ -722,7 +722,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -743,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -773,7 +773,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -782,7 +782,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -791,10 +791,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="J6" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
@@ -803,10 +803,10 @@
         <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
@@ -833,16 +833,16 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -854,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
@@ -863,10 +863,10 @@
         <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="O7" t="n">
         <v>0</v>
@@ -887,10 +887,10 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -923,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="M8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
         <v>0</v>
@@ -947,13 +947,13 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -962,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -971,10 +971,10 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J9" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
@@ -983,10 +983,10 @@
         <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O9" t="n">
         <v>0</v>
@@ -1007,13 +1007,13 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -1022,7 +1022,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -1034,19 +1034,19 @@
         <v>0</v>
       </c>
       <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" t="n">
         <v>16</v>
       </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M10" t="n">
-        <v>1</v>
-      </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O10" t="n">
         <v>0</v>
@@ -1067,10 +1067,10 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -1082,10 +1082,10 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1103,13 +1103,13 @@
         <v>1</v>
       </c>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" t="n">
         <v>0</v>
       </c>
       <c r="O11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
@@ -1127,13 +1127,13 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -1142,10 +1142,10 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1154,22 +1154,22 @@
         <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="L12" t="n">
         <v>1</v>
       </c>
       <c r="M12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="O12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12" t="inlineStr">
         <is>
@@ -1187,13 +1187,13 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -1202,10 +1202,10 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1214,7 +1214,7 @@
         <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
@@ -1223,13 +1223,13 @@
         <v>1</v>
       </c>
       <c r="M13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" t="inlineStr">
         <is>
@@ -1247,10 +1247,10 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -1259,13 +1259,13 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1277,19 +1277,19 @@
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" t="n">
         <v>1</v>
       </c>
       <c r="M14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>
@@ -1307,25 +1307,25 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1334,22 +1334,22 @@
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" t="n">
         <v>1</v>
       </c>
       <c r="M15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="O15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15" t="inlineStr">
         <is>
@@ -1367,25 +1367,25 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1394,22 +1394,22 @@
         <v>0</v>
       </c>
       <c r="J16" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" t="n">
         <v>1</v>
       </c>
       <c r="M16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="O16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" t="inlineStr">
         <is>
@@ -1427,10 +1427,10 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -1439,16 +1439,16 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1457,19 +1457,19 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L17" t="n">
         <v>1</v>
       </c>
       <c r="M17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17" t="inlineStr">
         <is>
@@ -1487,49 +1487,49 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18" t="n">
         <v>1</v>
       </c>
       <c r="M18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" t="inlineStr">
         <is>
@@ -1547,49 +1547,49 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
       </c>
       <c r="J19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" t="n">
         <v>1</v>
       </c>
       <c r="M19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="O19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P19" t="inlineStr">
         <is>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20" t="n">
         <v>1</v>
@@ -1619,16 +1619,16 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -1637,19 +1637,19 @@
         <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" t="n">
         <v>1</v>
       </c>
       <c r="M20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P20" t="inlineStr">
         <is>
@@ -1667,49 +1667,49 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21" t="n">
         <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L21" t="n">
         <v>1</v>
       </c>
       <c r="M21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="O21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P21" t="inlineStr">
         <is>
@@ -1727,49 +1727,49 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" t="n">
         <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L22" t="n">
         <v>1</v>
       </c>
       <c r="M22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="O22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P22" t="inlineStr">
         <is>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" t="n">
         <v>1</v>
@@ -1799,37 +1799,37 @@
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L23" t="n">
         <v>1</v>
       </c>
       <c r="M23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P23" t="inlineStr">
         <is>
@@ -1847,49 +1847,49 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" t="n">
         <v>1</v>
       </c>
       <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" t="n">
+        <v>45</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
+        <v>2</v>
+      </c>
+      <c r="L24" t="n">
+        <v>1</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
         <v>11</v>
       </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" t="n">
-        <v>1</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0</v>
-      </c>
-      <c r="I24" t="n">
-        <v>1</v>
-      </c>
-      <c r="J24" t="n">
-        <v>8</v>
-      </c>
-      <c r="K24" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" t="n">
-        <v>1</v>
-      </c>
-      <c r="M24" t="n">
-        <v>1</v>
-      </c>
-      <c r="N24" t="n">
-        <v>1</v>
-      </c>
       <c r="O24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P24" t="inlineStr">
         <is>
@@ -1907,49 +1907,49 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25" t="n">
         <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L25" t="n">
         <v>1</v>
       </c>
       <c r="M25" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="N25" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="O25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25" t="inlineStr">
         <is>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26" t="n">
         <v>1</v>
@@ -1976,40 +1976,40 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L26" t="n">
         <v>1</v>
       </c>
       <c r="M26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P26" t="inlineStr">
         <is>
@@ -2027,49 +2027,49 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" t="n">
         <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L27" t="n">
         <v>1</v>
       </c>
       <c r="M27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N27" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="O27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P27" t="inlineStr">
         <is>
@@ -2087,49 +2087,49 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C28" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L28" t="n">
         <v>1</v>
       </c>
       <c r="M28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N28" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="O28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P28" t="inlineStr">
         <is>
@@ -2147,10 +2147,10 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -2159,10 +2159,10 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
@@ -2171,25 +2171,25 @@
         <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29" t="n">
         <v>0</v>
       </c>
       <c r="L29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P29" t="inlineStr">
         <is>
@@ -2207,22 +2207,22 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
@@ -2231,25 +2231,25 @@
         <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K30" t="n">
         <v>0</v>
       </c>
       <c r="L30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N30" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="O30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P30" t="inlineStr">
         <is>
@@ -2267,22 +2267,22 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" t="n">
         <v>0</v>
@@ -2291,25 +2291,25 @@
         <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K31" t="n">
         <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N31" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="O31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P31" t="inlineStr">
         <is>
@@ -2327,10 +2327,10 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -2339,10 +2339,10 @@
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
@@ -2351,10 +2351,10 @@
         <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K32" t="n">
         <v>0</v>
@@ -2363,13 +2363,13 @@
         <v>1</v>
       </c>
       <c r="M32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P32" t="inlineStr">
         <is>
@@ -2387,49 +2387,49 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
+        <v>0</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>31</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>1</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
         <v>8</v>
       </c>
-      <c r="B33" t="n">
-        <v>1</v>
-      </c>
-      <c r="C33" t="n">
-        <v>45</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" t="n">
-        <v>3</v>
-      </c>
-      <c r="F33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" t="n">
-        <v>0</v>
-      </c>
-      <c r="I33" t="n">
-        <v>1</v>
-      </c>
-      <c r="J33" t="n">
-        <v>1</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" t="n">
-        <v>1</v>
-      </c>
-      <c r="M33" t="n">
-        <v>1</v>
-      </c>
-      <c r="N33" t="n">
-        <v>1</v>
-      </c>
       <c r="O33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P33" t="inlineStr">
         <is>
@@ -2447,22 +2447,22 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="B34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
@@ -2471,10 +2471,10 @@
         <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34" t="n">
         <v>0</v>
@@ -2483,13 +2483,13 @@
         <v>1</v>
       </c>
       <c r="M34" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="N34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P34" t="inlineStr">
         <is>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B35" t="n">
         <v>1</v>
@@ -2519,10 +2519,10 @@
         <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
@@ -2531,25 +2531,25 @@
         <v>0</v>
       </c>
       <c r="I35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L35" t="n">
         <v>1</v>
       </c>
       <c r="M35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P35" t="inlineStr">
         <is>
@@ -2567,49 +2567,49 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B36" t="n">
         <v>1</v>
       </c>
       <c r="C36" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L36" t="n">
         <v>1</v>
       </c>
       <c r="M36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N36" t="n">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="O36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P36" t="inlineStr">
         <is>
@@ -2627,49 +2627,49 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37" t="n">
         <v>1</v>
       </c>
       <c r="C37" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L37" t="n">
         <v>1</v>
       </c>
       <c r="M37" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="N37" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="O37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P37" t="inlineStr">
         <is>
@@ -2690,7 +2690,7 @@
         <v>0</v>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -2702,7 +2702,7 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
@@ -2714,7 +2714,7 @@
         <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" t="n">
         <v>0</v>
@@ -2750,10 +2750,10 @@
         <v>0</v>
       </c>
       <c r="B39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
@@ -2762,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G39" t="n">
         <v>0</v>
@@ -2774,7 +2774,7 @@
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K39" t="n">
         <v>0</v>
@@ -2786,7 +2786,7 @@
         <v>0</v>
       </c>
       <c r="N39" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="O39" t="n">
         <v>0</v>
@@ -2807,13 +2807,13 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
@@ -2822,7 +2822,7 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" t="n">
         <v>0</v>
@@ -2834,7 +2834,7 @@
         <v>0</v>
       </c>
       <c r="J40" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="K40" t="n">
         <v>0</v>
@@ -2846,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="N40" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="O40" t="n">
         <v>0</v>
@@ -2870,7 +2870,7 @@
         <v>0</v>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -2882,10 +2882,10 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" t="n">
         <v>0</v>
@@ -2894,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="J41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" t="n">
         <v>0</v>
@@ -2903,7 +2903,7 @@
         <v>1</v>
       </c>
       <c r="M41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N41" t="n">
         <v>0</v>
@@ -2930,10 +2930,10 @@
         <v>0</v>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C42" t="n">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D42" t="n">
         <v>0</v>
@@ -2942,10 +2942,10 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" t="n">
         <v>0</v>
@@ -2954,7 +2954,7 @@
         <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K42" t="n">
         <v>0</v>
@@ -2963,10 +2963,10 @@
         <v>1</v>
       </c>
       <c r="M42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N42" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O42" t="n">
         <v>0</v>
@@ -2990,10 +2990,10 @@
         <v>0</v>
       </c>
       <c r="B43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
         <v>0</v>
@@ -3002,10 +3002,10 @@
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
@@ -3014,19 +3014,19 @@
         <v>0</v>
       </c>
       <c r="J43" t="n">
+        <v>1</v>
+      </c>
+      <c r="K43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>18</v>
+      </c>
+      <c r="M43" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" t="n">
         <v>12</v>
-      </c>
-      <c r="K43" t="n">
-        <v>0</v>
-      </c>
-      <c r="L43" t="n">
-        <v>1</v>
-      </c>
-      <c r="M43" t="n">
-        <v>1</v>
-      </c>
-      <c r="N43" t="n">
-        <v>0</v>
       </c>
       <c r="O43" t="n">
         <v>0</v>
@@ -3047,10 +3047,10 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -3062,10 +3062,10 @@
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -3074,16 +3074,16 @@
         <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L44" t="n">
         <v>1</v>
       </c>
       <c r="M44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N44" t="n">
         <v>0</v>
@@ -3107,13 +3107,13 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
         <v>0</v>
@@ -3122,31 +3122,31 @@
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
       </c>
       <c r="J45" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="K45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L45" t="n">
         <v>1</v>
       </c>
       <c r="M45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N45" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O45" t="n">
         <v>0</v>
@@ -3167,13 +3167,13 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
@@ -3182,10 +3182,10 @@
         <v>0</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" t="n">
         <v>0</v>
@@ -3194,19 +3194,19 @@
         <v>0</v>
       </c>
       <c r="J46" t="n">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="K46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" t="n">
         <v>1</v>
       </c>
       <c r="M46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N46" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="O46" t="n">
         <v>0</v>
@@ -3227,10 +3227,10 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -3239,13 +3239,13 @@
         <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -3254,22 +3254,22 @@
         <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L47" t="n">
         <v>1</v>
       </c>
       <c r="M47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N47" t="n">
         <v>0</v>
       </c>
       <c r="O47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P47" t="inlineStr">
         <is>
@@ -3287,25 +3287,25 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
@@ -3314,22 +3314,22 @@
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="K48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L48" t="n">
         <v>1</v>
       </c>
       <c r="M48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N48" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="O48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P48" t="inlineStr">
         <is>
@@ -3347,25 +3347,25 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1</v>
+      </c>
+      <c r="F49" t="n">
         <v>33</v>
       </c>
-      <c r="D49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0</v>
-      </c>
-      <c r="F49" t="n">
-        <v>0</v>
-      </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49" t="n">
         <v>0</v>
@@ -3374,22 +3374,22 @@
         <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="K49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49" t="n">
         <v>1</v>
       </c>
       <c r="M49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N49" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P49" t="inlineStr">
         <is>
@@ -3407,10 +3407,10 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -3422,10 +3422,10 @@
         <v>1</v>
       </c>
       <c r="F50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" t="n">
         <v>0</v>
@@ -3434,10 +3434,10 @@
         <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L50" t="n">
         <v>1</v>
@@ -3449,7 +3449,7 @@
         <v>0</v>
       </c>
       <c r="O50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P50" t="inlineStr">
         <is>
@@ -3467,25 +3467,25 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D51" t="n">
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="F51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -3494,10 +3494,10 @@
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="K51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51" t="n">
         <v>1</v>
@@ -3506,10 +3506,10 @@
         <v>1</v>
       </c>
       <c r="N51" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P51" t="inlineStr">
         <is>
@@ -3527,13 +3527,13 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C52" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
@@ -3542,22 +3542,22 @@
         <v>1</v>
       </c>
       <c r="F52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" t="n">
         <v>0</v>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J52" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="K52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L52" t="n">
         <v>1</v>
@@ -3566,10 +3566,10 @@
         <v>1</v>
       </c>
       <c r="N52" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P52" t="inlineStr">
         <is>
@@ -3587,10 +3587,10 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
@@ -3602,22 +3602,22 @@
         <v>1</v>
       </c>
       <c r="F53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" t="n">
         <v>0</v>
       </c>
       <c r="J53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L53" t="n">
         <v>1</v>
@@ -3626,10 +3626,10 @@
         <v>1</v>
       </c>
       <c r="N53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P53" t="inlineStr">
         <is>
@@ -3647,13 +3647,13 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
@@ -3662,22 +3662,22 @@
         <v>1</v>
       </c>
       <c r="F54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J54" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="K54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L54" t="n">
         <v>1</v>
@@ -3686,10 +3686,10 @@
         <v>1</v>
       </c>
       <c r="N54" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="O54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P54" t="inlineStr">
         <is>
@@ -3707,13 +3707,13 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
@@ -3722,22 +3722,22 @@
         <v>1</v>
       </c>
       <c r="F55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" t="n">
         <v>0</v>
       </c>
       <c r="J55" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L55" t="n">
         <v>1</v>
@@ -3746,10 +3746,10 @@
         <v>1</v>
       </c>
       <c r="N55" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="O55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P55" t="inlineStr">
         <is>
@@ -3767,7 +3767,7 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B56" t="n">
         <v>1</v>
@@ -3782,22 +3782,22 @@
         <v>1</v>
       </c>
       <c r="F56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" t="n">
         <v>0</v>
       </c>
       <c r="J56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K56" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L56" t="n">
         <v>1</v>
@@ -3806,10 +3806,10 @@
         <v>1</v>
       </c>
       <c r="N56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P56" t="inlineStr">
         <is>
@@ -3827,13 +3827,13 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B57" t="n">
         <v>1</v>
       </c>
       <c r="C57" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D57" t="n">
         <v>0</v>
@@ -3842,22 +3842,22 @@
         <v>1</v>
       </c>
       <c r="F57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" t="n">
         <v>0</v>
       </c>
       <c r="J57" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="K57" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L57" t="n">
         <v>1</v>
@@ -3866,10 +3866,10 @@
         <v>1</v>
       </c>
       <c r="N57" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="O57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P57" t="inlineStr">
         <is>
@@ -3887,13 +3887,13 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B58" t="n">
         <v>1</v>
       </c>
       <c r="C58" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D58" t="n">
         <v>0</v>
@@ -3902,22 +3902,22 @@
         <v>1</v>
       </c>
       <c r="F58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58" t="n">
         <v>0</v>
       </c>
       <c r="J58" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="K58" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L58" t="n">
         <v>1</v>
@@ -3926,10 +3926,10 @@
         <v>1</v>
       </c>
       <c r="N58" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="O58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P58" t="inlineStr">
         <is>
@@ -3947,7 +3947,7 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B59" t="n">
         <v>1</v>
@@ -3956,28 +3956,28 @@
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" t="n">
         <v>1</v>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K59" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L59" t="n">
         <v>1</v>
@@ -3986,10 +3986,10 @@
         <v>1</v>
       </c>
       <c r="N59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P59" t="inlineStr">
         <is>
@@ -4007,37 +4007,37 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B60" t="n">
         <v>1</v>
       </c>
       <c r="C60" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="K60" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L60" t="n">
         <v>1</v>
@@ -4046,10 +4046,10 @@
         <v>1</v>
       </c>
       <c r="N60" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="O60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P60" t="inlineStr">
         <is>
@@ -4067,37 +4067,37 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B61" t="n">
         <v>1</v>
       </c>
       <c r="C61" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61" t="n">
         <v>1</v>
       </c>
       <c r="F61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" t="n">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="K61" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L61" t="n">
         <v>1</v>
@@ -4106,10 +4106,10 @@
         <v>1</v>
       </c>
       <c r="N61" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="O61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P61" t="inlineStr">
         <is>

</xml_diff>